<commit_message>
added extran version dates
</commit_message>
<xml_diff>
--- a/Notebooks/paycell_update_history_app_store.xlsx
+++ b/Notebooks/paycell_update_history_app_store.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismet bal\paycell-review-analysis\Notebooks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A006227F-AA3F-4B04-9D0B-97519353EDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="122">
   <si>
     <t>Date</t>
   </si>
@@ -23,81 +29,6 @@
   </si>
   <si>
     <t>Update</t>
-  </si>
-  <si>
-    <t>4 Tem 2025</t>
-  </si>
-  <si>
-    <t>25 Haz 2025</t>
-  </si>
-  <si>
-    <t>2 Haz 2025</t>
-  </si>
-  <si>
-    <t>29 May 2025</t>
-  </si>
-  <si>
-    <t>9 May 2025</t>
-  </si>
-  <si>
-    <t>28 Mar 2025</t>
-  </si>
-  <si>
-    <t>20 Mar 2025</t>
-  </si>
-  <si>
-    <t>11 Şub 2025</t>
-  </si>
-  <si>
-    <t>7 Şub 2025</t>
-  </si>
-  <si>
-    <t>28 Oca 2025</t>
-  </si>
-  <si>
-    <t>15 Oca 2025</t>
-  </si>
-  <si>
-    <t>12 Oca 2025</t>
-  </si>
-  <si>
-    <t>28 Kas 2024</t>
-  </si>
-  <si>
-    <t>26 Kas 2024</t>
-  </si>
-  <si>
-    <t>20 Kas 2024</t>
-  </si>
-  <si>
-    <t>15 Kas 2024</t>
-  </si>
-  <si>
-    <t>15 Eki 2024</t>
-  </si>
-  <si>
-    <t>4 Eki 2024</t>
-  </si>
-  <si>
-    <t>10 Eyl 2024</t>
-  </si>
-  <si>
-    <t>21 Ağu 2024</t>
-  </si>
-  <si>
-    <t>28 Haz 2024</t>
-  </si>
-  <si>
-    <t>6 Haz 2024</t>
-  </si>
-  <si>
-    <t>29 May 2024</t>
-  </si>
-  <si>
-    <t>14 May 2024</t>
-  </si>
-  <si>
-    <t>30 Nis 2024</t>
   </si>
   <si>
     <t>9.3.1</t>
@@ -264,12 +195,240 @@
     <t>Geleceğin finansal teknolojisi Paycell’i geliştirmeye devam ediyoruz. Bu sürümde deneyimini iyileştirmek için performans iyileştirmeleri yaptık.
 Türkiye'nin ilk ve tek yerli ödeme sistemi olan Troy Paycell kartlarını oluşturabilir, harcamalarında ve para transferlerinde kullanabilirsin. Uygulamaya giriş yapmadan sana özel kampanyalara katılım sağlayabilir, ödemeler alanında Turkcell ve birçok farklı kurum faturanı kolayca ödeyebilirsin. Tüm bu yenilikler için uygulamanı güncellemeyi unutma!</t>
   </si>
+  <si>
+    <t>7.7.2</t>
+  </si>
+  <si>
+    <t>7.7.1</t>
+  </si>
+  <si>
+    <t>7.7.0</t>
+  </si>
+  <si>
+    <t>7.6.2</t>
+  </si>
+  <si>
+    <t>7.6.1</t>
+  </si>
+  <si>
+    <t>7.6.0</t>
+  </si>
+  <si>
+    <t>7.5.0</t>
+  </si>
+  <si>
+    <t>7.4.3</t>
+  </si>
+  <si>
+    <t>7.4.2</t>
+  </si>
+  <si>
+    <t>7.4.1</t>
+  </si>
+  <si>
+    <t>7.4.0</t>
+  </si>
+  <si>
+    <t>7.3.2</t>
+  </si>
+  <si>
+    <t>7.3.1</t>
+  </si>
+  <si>
+    <t>7.3.0</t>
+  </si>
+  <si>
+    <t>7.2.1</t>
+  </si>
+  <si>
+    <t>7.1.3</t>
+  </si>
+  <si>
+    <t>7.1.2</t>
+  </si>
+  <si>
+    <t>7.1.1</t>
+  </si>
+  <si>
+    <t>7.1.0</t>
+  </si>
+  <si>
+    <t>6.7.2</t>
+  </si>
+  <si>
+    <t>6.5.3</t>
+  </si>
+  <si>
+    <t>6.5.2</t>
+  </si>
+  <si>
+    <t>6.5.1</t>
+  </si>
+  <si>
+    <t>6.4.4</t>
+  </si>
+  <si>
+    <t>6.4.1</t>
+  </si>
+  <si>
+    <t>Türkiye'nin ilk ve tek yerli ödeme sistemi Troy Paycell kartlarını oluşturabilir, harcamalarınızda ve para transferlerinizde kullanabilirsiniz. Uygulamaya giriş yapmadan size özel kampanyalara katılarak avantajlardan yararlanabilirsiniz. Ödemeler alanında tüm Turkcell faturalarını sorgulayabilir, yenilenen ödeme deneyimi ile birçok kurumsal faturayı kolayca ödeyebilirsiniz.</t>
+  </si>
+  <si>
+    <t>Bu sürümde, hayatın akışı içinde ihtiyaç duyduğunuz yeni finansal teknolojileri ekledik ve çeşitli hata düzeltmeleri ve performans ayarlamaları yaptık.</t>
+  </si>
+  <si>
+    <t>İşlemlerinizi daha kolay ve hızlı tamamlayabilmeniz için Paycell'in menü ve sayfalarını güncelleyerek yepyeni bir arayüzle sizlere sunuyoruz.</t>
+  </si>
+  <si>
+    <t>We've made some improvements to serve you better.</t>
+  </si>
+  <si>
+    <t>25-06-2025</t>
+  </si>
+  <si>
+    <t>04-07-2025</t>
+  </si>
+  <si>
+    <t>2-06-2025</t>
+  </si>
+  <si>
+    <t>29-05-2025</t>
+  </si>
+  <si>
+    <t>9-05-2025</t>
+  </si>
+  <si>
+    <t>28-03-2025</t>
+  </si>
+  <si>
+    <t>20-03-2025</t>
+  </si>
+  <si>
+    <t>11-02-2025</t>
+  </si>
+  <si>
+    <t>7-02-2025</t>
+  </si>
+  <si>
+    <t>28-01-2025</t>
+  </si>
+  <si>
+    <t>15-01-2025</t>
+  </si>
+  <si>
+    <t>12-01-2025</t>
+  </si>
+  <si>
+    <t>28-11-2024</t>
+  </si>
+  <si>
+    <t>26-11-2024</t>
+  </si>
+  <si>
+    <t>20-11-2024</t>
+  </si>
+  <si>
+    <t>15-11-2024</t>
+  </si>
+  <si>
+    <t>15-10-2024</t>
+  </si>
+  <si>
+    <t>4-10-2024</t>
+  </si>
+  <si>
+    <t>10-09-2024</t>
+  </si>
+  <si>
+    <t>21-08-2024</t>
+  </si>
+  <si>
+    <t>28-06-2024</t>
+  </si>
+  <si>
+    <t>6-06-2024</t>
+  </si>
+  <si>
+    <t>29-05-2024</t>
+  </si>
+  <si>
+    <t>14-05-2024</t>
+  </si>
+  <si>
+    <t>30-04-2024</t>
+  </si>
+  <si>
+    <t>29-03-2024</t>
+  </si>
+  <si>
+    <t>12-03-2024</t>
+  </si>
+  <si>
+    <t>6-03-2024</t>
+  </si>
+  <si>
+    <t>13-01-2024</t>
+  </si>
+  <si>
+    <t>8-01-2024</t>
+  </si>
+  <si>
+    <t>1-01-2024</t>
+  </si>
+  <si>
+    <t>15-12-2023</t>
+  </si>
+  <si>
+    <t>14-11-2023</t>
+  </si>
+  <si>
+    <t>12-11-2023</t>
+  </si>
+  <si>
+    <t>7-11-2023</t>
+  </si>
+  <si>
+    <t>5-11-2023</t>
+  </si>
+  <si>
+    <t>20-10-2023</t>
+  </si>
+  <si>
+    <t>10-09-2023</t>
+  </si>
+  <si>
+    <t>29-07-2023</t>
+  </si>
+  <si>
+    <t>26-07-2023</t>
+  </si>
+  <si>
+    <t>19-07-2023</t>
+  </si>
+  <si>
+    <t>28-06-2023</t>
+  </si>
+  <si>
+    <t>11-06-2023</t>
+  </si>
+  <si>
+    <t>9-04-2023</t>
+  </si>
+  <si>
+    <t>22-03-2023</t>
+  </si>
+  <si>
+    <t>8-03-2023</t>
+  </si>
+  <si>
+    <t>18-01-2023</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,24 +480,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -376,7 +546,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -410,6 +580,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -444,9 +615,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -619,14 +791,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" customWidth="1"/>
+    <col min="3" max="3" width="167.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -637,279 +816,521 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="C39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="C41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="C42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="C43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="C44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="C45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="C46" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="C49" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="C50" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" t="s">
-        <v>70</v>
+      <c r="C51" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update history new datas found
</commit_message>
<xml_diff>
--- a/Notebooks/paycell_update_history_app_store.xlsx
+++ b/Notebooks/paycell_update_history_app_store.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismet bal\paycell-review-analysis\Notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A006227F-AA3F-4B04-9D0B-97519353EDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8499121E-1669-4A08-B892-06C2983DB816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="137">
   <si>
     <t>Date</t>
   </si>
@@ -409,9 +409,6 @@
     <t>28-06-2023</t>
   </si>
   <si>
-    <t>11-06-2023</t>
-  </si>
-  <si>
     <t>9-04-2023</t>
   </si>
   <si>
@@ -421,7 +418,55 @@
     <t>8-03-2023</t>
   </si>
   <si>
-    <t>18-01-2023</t>
+    <t>6.2.0</t>
+  </si>
+  <si>
+    <t>6.0.1</t>
+  </si>
+  <si>
+    <t>6.0.0</t>
+  </si>
+  <si>
+    <t>5.9.0</t>
+  </si>
+  <si>
+    <t>22-12-2022</t>
+  </si>
+  <si>
+    <t>12-08-2022</t>
+  </si>
+  <si>
+    <t>19-09-2022</t>
+  </si>
+  <si>
+    <t>23-09-2022</t>
+  </si>
+  <si>
+    <t>22-11-2022</t>
+  </si>
+  <si>
+    <t>25-01-2023</t>
+  </si>
+  <si>
+    <t>26-05-2023</t>
+  </si>
+  <si>
+    <t>16-05-2023</t>
+  </si>
+  <si>
+    <t>6.7.1</t>
+  </si>
+  <si>
+    <t>3-05-2023</t>
+  </si>
+  <si>
+    <t>6.7.0</t>
+  </si>
+  <si>
+    <t>18-04-2023</t>
+  </si>
+  <si>
+    <t>6.6.0</t>
   </si>
 </sst>
 </file>
@@ -480,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -488,6 +533,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -792,17 +840,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="5.88671875" customWidth="1"/>
-    <col min="3" max="3" width="167.77734375" customWidth="1"/>
+    <col min="3" max="3" width="255.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -937,47 +985,47 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1003,36 +1051,36 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1275,7 +1323,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>65</v>
@@ -1286,51 +1334,107 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>67</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C49" t="s">
-        <v>74</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C50" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C51" t="s">
-        <v>74</v>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>